<commit_message>
Fixes and new results
</commit_message>
<xml_diff>
--- a/test/HammingTestingResult.xlsx
+++ b/test/HammingTestingResult.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikolaj/Documents/Repositories/HammingCodes/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E7B9422-A869-9449-BB4D-BF1DD7935E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA19EEB-81F8-D449-A83E-FEA11BD20FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{9CC900A8-12C8-6D4A-90A7-896FC5B8A195}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>size: 4096</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t>PB count/WN percent</t>
+  </si>
+  <si>
+    <t>PB/Size</t>
+  </si>
+  <si>
+    <t>ENC</t>
+  </si>
+  <si>
+    <t>DEC</t>
   </si>
 </sst>
 </file>
@@ -67,7 +76,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -75,12 +84,103 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1210,7 +1310,919 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$49:$B$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.5999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F48C-1048-810E-3E0437669DEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$49:$C$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6.8000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F48C-1048-810E-3E0437669DEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$49:$D$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4000000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F48C-1048-810E-3E0437669DEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="199585999"/>
+        <c:axId val="199569519"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="199585999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="199569519"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="199569519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="199585999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$49:$G$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.2000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B438-2C49-8D3F-A43DA3997B49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$49:$H$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B438-2C49-8D3F-A43DA3997B49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$49:$I$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B438-2C49-8D3F-A43DA3997B49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="142873119"/>
+        <c:axId val="142874767"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="142873119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="142874767"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="142874767"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="142873119"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1766,6 +2778,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1799,6 +3843,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33687D2F-49D1-DD60-3AF5-963D598E5442}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>806450</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{202C4B6A-4CBD-FE92-84E5-40204ED456BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2104,10 +4220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB86A88D-CA02-C545-9C84-BEA8F50FE266}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2436,6 +4552,254 @@
         <v>50.56</v>
       </c>
     </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="3"/>
+      <c r="F47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="5">
+        <v>4096</v>
+      </c>
+      <c r="C48" s="5">
+        <v>8192</v>
+      </c>
+      <c r="D48" s="6">
+        <v>16384</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G48" s="5">
+        <v>4096</v>
+      </c>
+      <c r="H48" s="5">
+        <v>8192</v>
+      </c>
+      <c r="I48" s="6">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <v>2</v>
+      </c>
+      <c r="B49" s="5">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="C49" s="5">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="D49" s="6">
+        <v>0.16</v>
+      </c>
+      <c r="F49" s="4">
+        <v>2</v>
+      </c>
+      <c r="G49" s="5">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="H49" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="I49" s="6">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>3</v>
+      </c>
+      <c r="B50" s="5">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C50" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="D50" s="6">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="F50" s="4">
+        <v>3</v>
+      </c>
+      <c r="G50" s="5">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H50" s="10">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="I50" s="6">
+        <v>7.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <v>4</v>
+      </c>
+      <c r="B51" s="10">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C51" s="10">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D51" s="6">
+        <v>6.3E-2</v>
+      </c>
+      <c r="F51" s="4">
+        <v>4</v>
+      </c>
+      <c r="G51" s="10">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H51" s="10">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="I51" s="6">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>5</v>
+      </c>
+      <c r="B52" s="10">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C52" s="10">
+        <v>3.1E-2</v>
+      </c>
+      <c r="D52" s="6">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="F52" s="4">
+        <v>5</v>
+      </c>
+      <c r="G52" s="10">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="H52" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="I52" s="6">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
+        <v>6</v>
+      </c>
+      <c r="B53" s="10">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C53" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D53" s="6">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="F53" s="4">
+        <v>6</v>
+      </c>
+      <c r="G53" s="10">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H53" s="10">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="I53" s="6">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
+        <v>7</v>
+      </c>
+      <c r="B54" s="10">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C54" s="10">
+        <v>3.1E-2</v>
+      </c>
+      <c r="D54" s="6">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F54" s="4">
+        <v>7</v>
+      </c>
+      <c r="G54" s="10">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="H54" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="I54" s="6">
+        <v>6.2E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
+        <v>8</v>
+      </c>
+      <c r="B55" s="10">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C55" s="10">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D55" s="6">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F55" s="4">
+        <v>8</v>
+      </c>
+      <c r="G55" s="10">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="H55" s="10">
+        <v>3.1E-2</v>
+      </c>
+      <c r="I55" s="6">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="7">
+        <v>9</v>
+      </c>
+      <c r="B56" s="11">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C56" s="8">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D56" s="9">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="F56" s="7">
+        <v>9</v>
+      </c>
+      <c r="G56" s="11">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H56" s="8">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="I56" s="9">
+        <v>6.3E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>